<commit_message>
Add test for empty evaluation in an empty sheet
</commit_message>
<xml_diff>
--- a/tests/ast/basic_evaluation.xlsx
+++ b/tests/ast/basic_evaluation.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\workspace\koala\tests\ast\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D50AFFC-774D-4F86-826B-7B6BF0EC3CC6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{319D0870-DAAA-477D-8536-B36D10034573}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="EmptyRange">Sheet1!$A$12:$G$12</definedName>
@@ -499,8 +500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1037,6 +1038,10 @@
         <v>1</v>
       </c>
       <c r="C36" t="s">
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <f>Sheet3!AA59</f>
         <v>0</v>
       </c>
     </row>
@@ -1198,4 +1203,18 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DC58497-A0F0-4A64-897F-CAE5CC493DE9}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView topLeftCell="B28" workbookViewId="0">
+      <selection activeCell="X59" sqref="X59"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>